<commit_message>
removed network nav bar
</commit_message>
<xml_diff>
--- a/Poets dataset.xlsx
+++ b/Poets dataset.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\peponi lyric map\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24560" windowHeight="13780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Places #" sheetId="1" r:id="rId1"/>
     <sheet name="Dataset proper" sheetId="2" r:id="rId2"/>
     <sheet name="Movement vectors" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -878,7 +878,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -913,7 +913,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1128,28 +1128,28 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="17.140625" style="5"/>
-    <col min="9" max="9" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="17.1640625" style="5"/>
+    <col min="9" max="9" width="6.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="12.75" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="12.75" customHeight="1">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="12.75" customHeight="1">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="12.75" customHeight="1">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="12.75" customHeight="1">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" ht="12.75" customHeight="1">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="12.75" customHeight="1">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" ht="12.75" customHeight="1">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="12.75" customHeight="1">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="12.75" customHeight="1">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" ht="12.75" customHeight="1">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="12.75" customHeight="1">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" ht="12.75" customHeight="1">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" ht="12.75" customHeight="1">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" ht="12.75" customHeight="1">
       <c r="A15" t="s">
         <v>148</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" ht="12.75" customHeight="1">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" ht="12.75" customHeight="1">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" ht="12.75" customHeight="1">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" ht="12.75" customHeight="1">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" ht="12.75" customHeight="1">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" ht="12.75" customHeight="1">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" ht="12.75" customHeight="1">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" ht="12.75" customHeight="1">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" ht="12.75" customHeight="1">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" ht="12.75" customHeight="1">
       <c r="A25" t="s">
         <v>149</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" ht="12.75" customHeight="1">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" ht="12.75" customHeight="1">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" ht="12.75" customHeight="1">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" ht="12.75" customHeight="1">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" ht="12.75" customHeight="1">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" ht="12.75" customHeight="1">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" ht="12.75" customHeight="1">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" ht="24">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" ht="24">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" ht="12.75" customHeight="1">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -4189,8 +4189,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4199,24 +4204,24 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.42578125" customWidth="1"/>
+    <col min="8" max="8" width="60.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -4245,7 +4250,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12.75" customHeight="1">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -4275,7 +4280,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="12.75" customHeight="1">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -4302,7 +4307,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="12.75" customHeight="1">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -4326,7 +4331,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -4350,7 +4355,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="12.75" customHeight="1">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -4377,7 +4382,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="12.75" customHeight="1">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -4407,7 +4412,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="12.75" customHeight="1">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -4434,7 +4439,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -4458,7 +4463,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="12.75" customHeight="1">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -4479,7 +4484,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="12.75" customHeight="1">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -4503,7 +4508,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -4527,7 +4532,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -4551,7 +4556,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -4572,7 +4577,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="12.75" customHeight="1">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -4596,7 +4601,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="12.75" customHeight="1">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -4617,7 +4622,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="12.75" customHeight="1">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -4638,7 +4643,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="12.75" customHeight="1">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -4659,7 +4664,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="12.75" customHeight="1">
       <c r="A19" t="s">
         <v>80</v>
       </c>
@@ -4680,7 +4685,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="24">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -4704,7 +4709,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="24">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -4728,7 +4733,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="12">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -4749,7 +4754,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="12">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -4773,7 +4778,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="12">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -4797,7 +4802,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="24">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -4824,7 +4829,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="12">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -4845,7 +4850,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="12">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -4869,7 +4874,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="12">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -4890,7 +4895,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="12">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -4908,7 +4913,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="12">
       <c r="A30" t="s">
         <v>105</v>
       </c>
@@ -4932,7 +4937,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="12">
       <c r="A31" t="s">
         <v>106</v>
       </c>
@@ -4953,7 +4958,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="12">
       <c r="A32" t="s">
         <v>107</v>
       </c>
@@ -4980,7 +4985,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="12">
       <c r="A33" t="s">
         <v>109</v>
       </c>
@@ -4998,7 +5003,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="12">
       <c r="A34" t="s">
         <v>111</v>
       </c>
@@ -5016,7 +5021,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="12">
       <c r="A35" t="s">
         <v>112</v>
       </c>
@@ -5031,7 +5036,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="12">
       <c r="A36" t="s">
         <v>113</v>
       </c>
@@ -5052,7 +5057,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="12">
       <c r="A37" t="s">
         <v>116</v>
       </c>
@@ -5076,7 +5081,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="12">
       <c r="A38" t="s">
         <v>119</v>
       </c>
@@ -5100,7 +5105,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="12">
       <c r="A39" t="s">
         <v>121</v>
       </c>
@@ -5121,7 +5126,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="12">
       <c r="A40" t="s">
         <v>123</v>
       </c>
@@ -5142,7 +5147,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="12">
       <c r="A41" t="s">
         <v>125</v>
       </c>
@@ -5160,7 +5165,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="12">
       <c r="A42" t="s">
         <v>127</v>
       </c>
@@ -5181,7 +5186,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="12">
       <c r="A43" t="s">
         <v>129</v>
       </c>
@@ -5202,7 +5207,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="12">
       <c r="A44" t="s">
         <v>130</v>
       </c>
@@ -5226,7 +5231,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="12">
       <c r="A45" t="s">
         <v>132</v>
       </c>
@@ -5250,7 +5255,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="12">
       <c r="A46" t="s">
         <v>134</v>
       </c>
@@ -5274,7 +5279,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="12">
       <c r="A47" t="s">
         <v>136</v>
       </c>
@@ -5298,7 +5303,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="12">
       <c r="A48" t="s">
         <v>138</v>
       </c>
@@ -5322,7 +5327,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="12">
       <c r="A49" t="s">
         <v>140</v>
       </c>
@@ -5346,7 +5351,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="12">
       <c r="A50" t="s">
         <v>142</v>
       </c>
@@ -5367,7 +5372,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="12">
       <c r="A51" t="s">
         <v>144</v>
       </c>
@@ -5385,7 +5390,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="12">
       <c r="A52" t="s">
         <v>146</v>
       </c>
@@ -5411,7 +5416,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5424,12 +5434,12 @@
       <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -5443,13 +5453,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="12.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="12.75" customHeight="1">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -5463,7 +5473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="12.75" customHeight="1">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -5474,12 +5484,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="12.75" customHeight="1">
       <c r="D5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="12.75" customHeight="1">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -5490,7 +5500,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="12.75" customHeight="1">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -5501,7 +5511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="12.75" customHeight="1">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -5512,7 +5522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="12.75" customHeight="1">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -5526,17 +5536,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="12.75" customHeight="1">
       <c r="D10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="12.75" customHeight="1">
       <c r="D11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="12.75" customHeight="1">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -5547,17 +5557,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="12.75" customHeight="1">
       <c r="D13" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="12.75" customHeight="1">
       <c r="D14" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="12.75" customHeight="1">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -5568,7 +5578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="12.75" customHeight="1">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -5576,7 +5586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="12.75" customHeight="1">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -5587,7 +5597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="12.75" customHeight="1">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -5598,7 +5608,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="12.75" customHeight="1">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -5609,7 +5619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="12.75" customHeight="1">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -5617,7 +5627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="12.75" customHeight="1">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -5628,7 +5638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="12.75" customHeight="1">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -5636,7 +5646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="12.75" customHeight="1">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -5644,7 +5654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="12.75" customHeight="1">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -5652,7 +5662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="12">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -5663,7 +5673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="12">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -5674,7 +5684,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="12">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -5685,7 +5695,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="12">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -5693,7 +5703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="12">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -5701,7 +5711,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="12">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -5712,7 +5722,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="24">
       <c r="A31" t="s">
         <v>95</v>
       </c>
@@ -5726,22 +5736,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="12">
       <c r="D32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="12">
       <c r="D33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="12">
       <c r="D34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="12">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -5749,7 +5759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="12">
       <c r="A36" t="s">
         <v>99</v>
       </c>
@@ -5760,7 +5770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="12">
       <c r="A37" t="s">
         <v>100</v>
       </c>
@@ -5768,7 +5778,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="12">
       <c r="A38" t="s">
         <v>103</v>
       </c>
@@ -5776,7 +5786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="12">
       <c r="A39" t="s">
         <v>105</v>
       </c>
@@ -5784,7 +5794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="12">
       <c r="A40" t="s">
         <v>106</v>
       </c>
@@ -5795,12 +5805,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="24">
       <c r="D41" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="12">
       <c r="A42" t="s">
         <v>107</v>
       </c>
@@ -5814,12 +5824,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="12">
       <c r="A43" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="24">
       <c r="A44" t="s">
         <v>111</v>
       </c>
@@ -5827,12 +5837,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="12">
       <c r="A45" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="12">
       <c r="A46" t="s">
         <v>113</v>
       </c>
@@ -5840,22 +5850,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="12">
       <c r="D47" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="12">
       <c r="D48" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="12">
       <c r="D49" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="12">
       <c r="A50" t="s">
         <v>116</v>
       </c>
@@ -5866,17 +5876,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="12">
       <c r="D51" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="12">
       <c r="D52" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="12">
       <c r="A53" t="s">
         <v>119</v>
       </c>
@@ -5887,7 +5897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="12">
       <c r="A54" t="s">
         <v>121</v>
       </c>
@@ -5895,7 +5905,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="12">
       <c r="A55" t="s">
         <v>123</v>
       </c>
@@ -5903,12 +5913,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="12">
       <c r="A56" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="12">
       <c r="A57" t="s">
         <v>127</v>
       </c>
@@ -5916,7 +5926,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="12">
       <c r="A58" t="s">
         <v>129</v>
       </c>
@@ -5927,12 +5937,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="12">
       <c r="D59" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="12">
       <c r="A60" t="s">
         <v>130</v>
       </c>
@@ -5943,7 +5953,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="12">
       <c r="A61" t="s">
         <v>132</v>
       </c>
@@ -5954,7 +5964,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="12">
       <c r="A62" t="s">
         <v>134</v>
       </c>
@@ -5965,7 +5975,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="12">
       <c r="A63" t="s">
         <v>136</v>
       </c>
@@ -5976,7 +5986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="12">
       <c r="A64" t="s">
         <v>138</v>
       </c>
@@ -5987,7 +5997,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="12">
       <c r="A65" t="s">
         <v>140</v>
       </c>
@@ -5998,7 +6008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="12">
       <c r="A66" t="s">
         <v>142</v>
       </c>
@@ -6006,7 +6016,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="12">
       <c r="A67" t="s">
         <v>146</v>
       </c>
@@ -6017,12 +6027,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="12">
       <c r="D68" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>